<commit_message>
burndown 1 used doge
</commit_message>
<xml_diff>
--- a/Documentation/Burndown Chart Sprint 1 Complete.xlsx
+++ b/Documentation/Burndown Chart Sprint 1 Complete.xlsx
@@ -218,6 +218,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -230,13 +237,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1030,19 +1030,19 @@
                   <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>16</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>16</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>16</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>16</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>16</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1156,19 +1156,19 @@
                   <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>16</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>16</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>16</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>16</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>16</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1282,19 +1282,19 @@
                   <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>16</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>16</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>16</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>16</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>16</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1405,19 +1405,19 @@
                   <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>80</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>80</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>80</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>80</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>80</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1475,19 +1475,19 @@
                   <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>16</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>16</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>16</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>16</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>16</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1504,11 +1504,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-998039728"/>
-        <c:axId val="-998033200"/>
+        <c:axId val="1135598192"/>
+        <c:axId val="1135597104"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-998039728"/>
+        <c:axId val="1135598192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1519,7 +1519,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-998033200"/>
+        <c:crossAx val="1135597104"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1527,7 +1527,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-998033200"/>
+        <c:axId val="1135597104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1557,7 +1557,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-998039728"/>
+        <c:crossAx val="1135598192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1904,7 +1904,7 @@
   <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S22" sqref="S22"/>
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1913,75 +1913,75 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="6"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="11"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="8">
+      <c r="A2" s="4">
         <v>2014</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="10">
+      <c r="C2" s="6">
         <v>41712</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2" s="5">
         <v>41713</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="5">
         <v>41714</v>
       </c>
-      <c r="F2" s="9">
+      <c r="F2" s="5">
         <v>41715</v>
       </c>
-      <c r="G2" s="9">
+      <c r="G2" s="5">
         <v>41716</v>
       </c>
-      <c r="H2" s="10">
+      <c r="H2" s="6">
         <v>41717</v>
       </c>
-      <c r="I2" s="9">
+      <c r="I2" s="5">
         <v>41718</v>
       </c>
-      <c r="J2" s="9">
+      <c r="J2" s="5">
         <v>41719</v>
       </c>
-      <c r="K2" s="9">
+      <c r="K2" s="5">
         <v>41720</v>
       </c>
-      <c r="L2" s="9">
+      <c r="L2" s="5">
         <v>41721</v>
       </c>
-      <c r="M2" s="9">
+      <c r="M2" s="5">
         <v>41722</v>
       </c>
-      <c r="N2" s="9">
+      <c r="N2" s="5">
         <v>41723</v>
       </c>
-      <c r="O2" s="9">
+      <c r="O2" s="5">
         <v>41724</v>
       </c>
-      <c r="P2" s="9">
+      <c r="P2" s="5">
         <v>41725</v>
       </c>
-      <c r="Q2" s="11">
+      <c r="Q2" s="7">
         <v>41726</v>
       </c>
     </row>
@@ -2285,22 +2285,22 @@
         <v>16</v>
       </c>
       <c r="L8" s="1">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="M8" s="1">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="N8" s="1">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="O8" s="1">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="P8" s="1">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="Q8" s="1">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -2338,22 +2338,22 @@
         <v>16</v>
       </c>
       <c r="L9" s="1">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="M9" s="1">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="N9" s="1">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="O9" s="1">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="P9" s="1">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="Q9" s="1">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -2391,26 +2391,26 @@
         <v>16</v>
       </c>
       <c r="L10" s="1">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="M10" s="1">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="N10" s="1">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="O10" s="1">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="P10" s="1">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="Q10" s="1">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -2444,26 +2444,26 @@
         <v>16</v>
       </c>
       <c r="L11" s="1">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="M11" s="1">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="N11" s="1">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="O11" s="1">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="P11" s="1">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="Q11" s="1">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -2497,22 +2497,22 @@
         <v>16</v>
       </c>
       <c r="L12" s="1">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="M12" s="1">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="N12" s="1">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="O12" s="1">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="P12" s="1">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="Q12" s="1">
-        <v>16</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2558,27 +2558,27 @@
       </c>
       <c r="L13" s="2">
         <f t="shared" si="0"/>
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="M13" s="2">
         <f t="shared" si="0"/>
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="N13" s="2">
         <f t="shared" si="0"/>
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="O13" s="2">
         <f t="shared" si="0"/>
-        <v>80</v>
+        <v>25</v>
       </c>
       <c r="P13" s="2">
         <f t="shared" si="0"/>
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="Q13" s="2">
         <f t="shared" si="0"/>
-        <v>80</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>